<commit_message>
Ultimo javadoc, jar, classdiagram e dianusauro
</commit_message>
<xml_diff>
--- a/UML/CRC_Cards.xlsx
+++ b/UML/CRC_Cards.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t xml:space="preserve">CRC_CARDS</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fornisce il modello che soddisfa l’espressione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fornisce il numero di iterazioni eseguite</t>
   </si>
   <si>
     <r>
@@ -359,28 +362,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Superclasses </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ChronologicalTableau</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Configura il file di Log</t>
   </si>
   <si>
@@ -471,7 +452,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Carica il concetto previa selezione e ne verifica la soddisfacibilità</t>
+    <t xml:space="preserve">Carica il concetto da verificare previa selezione</t>
   </si>
   <si>
     <t xml:space="preserve">Java Swing</t>
@@ -483,6 +464,9 @@
     <t xml:space="preserve">Permette di lanciare una batteria di test</t>
   </si>
   <si>
+    <t xml:space="preserve">Visualizza i risultati della verifica</t>
+  </si>
+  <si>
     <t xml:space="preserve">Battery</t>
   </si>
   <si>
@@ -515,7 +499,7 @@
     <t xml:space="preserve">Carica ad uno ad uno tutti i concetti presenti nella cartella “Ontologie” e ne verifica la soddisfacibilità </t>
   </si>
   <si>
-    <t xml:space="preserve">Permette di visualizzare i file di Log dei concetti precedentemente verifificati</t>
+    <t xml:space="preserve">Imposta i file di log per il tracciamento dell’esecuzione</t>
   </si>
 </sst>
 </file>
@@ -525,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -563,12 +547,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -641,7 +619,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,11 +664,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -711,13 +685,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73:B83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.16"/>
@@ -901,15 +875,19 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -919,17 +897,17 @@
       </c>
       <c r="B34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B35" s="8"/>
       <c r="E35" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -955,7 +933,7 @@
     </row>
     <row r="38" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>17</v>
@@ -1005,13 +983,21 @@
       </c>
       <c r="F41" s="5"/>
     </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -1021,7 +1007,7 @@
       </c>
       <c r="B45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -1063,7 +1049,7 @@
         <v>34</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>17</v>
@@ -1094,6 +1080,11 @@
         <v>23</v>
       </c>
       <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
@@ -1252,84 +1243,83 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5" t="s">
-        <v>21</v>
+      <c r="A81" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11" t="s">
-        <v>47</v>
+      <c r="B82" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
-        <v>48</v>
-      </c>
+      <c r="A83" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" s="2"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
+      <c r="A87" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B89" s="12" t="s">
+    <row r="88" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="6"/>
-      <c r="B91" s="12" t="s">
-        <v>21</v>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="11"/>
-      <c r="B93" s="11"/>
-    </row>
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="48">
     <mergeCell ref="A3:B3"/>
@@ -1376,10 +1366,10 @@
     <mergeCell ref="A74:B74"/>
     <mergeCell ref="A75:B75"/>
     <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A83:B83"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>